<commit_message>
Update IP - EX 06 - Atalhos do excel  colar especial (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 06 - Atalhos do excel  colar especial (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 06 - Atalhos do excel  colar especial (Anexo).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF19795-C50A-4D85-957A-00C7828028E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264CC214-18AB-4CE1-B108-5FBF066801AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>

</xml_diff>